<commit_message>
Document purpose of spreadsheet 6, used in XSSFTabularDataSourceSpec and StreamingXSSFTabularDataSourceSpec a little better.  Spreadsheet 6 contains numeric with decimal portion, and a date, both susceptible to parsing issues.
</commit_message>
<xml_diff>
--- a/src/test/resources/xssf/spreadsheet6.xlsx
+++ b/src/test/resources/xssf/spreadsheet6.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="69280" yWindow="920" windowWidth="25040" windowHeight="15500" tabRatio="249"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="249"/>
   </bookViews>
   <sheets>
     <sheet name="One" sheetId="4" r:id="rId1"/>
@@ -24,13 +24,13 @@
     <t>Column A</t>
   </si>
   <si>
-    <t>Column B</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
-    <t>Column C</t>
+    <t>Date Data</t>
+  </si>
+  <si>
+    <t>Numeric Data With Decimal</t>
   </si>
 </sst>
 </file>
@@ -78,8 +78,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -95,17 +97,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -438,7 +442,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -451,15 +455,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>21212.4444</v>

</xml_diff>